<commit_message>
add new Proj Name : A3_6009A , A3_N609A , A3_8009  and A3_N609A_v3.0.p1 release
</commit_message>
<xml_diff>
--- a/doc/6009A/6009A_水表功能列表.xlsx
+++ b/doc/6009A/6009A_水表功能列表.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="3495" yWindow="720" windowWidth="17280" windowHeight="10590"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="348">
   <si>
     <t>表端</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1248,10 +1248,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>开始升级：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>step 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1264,10 +1260,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>查询升级状态：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>unknown         --&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1325,10 +1317,6 @@
   </si>
   <si>
     <t xml:space="preserve">  error     --&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  limit     --&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1446,12 +1434,52 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>模块应答结果：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  forbid    --&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升级状态：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升级步骤：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>跳转：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新当前状态：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入步骤前状态：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2、查询升级状态命令：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、开始升级命令 (初始状态可为如下任意)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升级过程简化为如下两个命令：（即 开始升级 和 查询升级状态， 其他过程自动识别并执行）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1569,8 +1597,23 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1592,6 +1635,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1740,7 +1795,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1776,6 +1831,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1813,7 +1871,7 @@
         <xdr:cNvPr id="3" name="直接箭头连接符 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1866,7 +1924,7 @@
         <xdr:cNvPr id="5" name="直接箭头连接符 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1919,7 +1977,7 @@
         <xdr:cNvPr id="7" name="直接箭头连接符 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1972,7 +2030,7 @@
         <xdr:cNvPr id="12" name="直接箭头连接符 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2025,7 +2083,7 @@
         <xdr:cNvPr id="14" name="直接箭头连接符 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2078,7 +2136,7 @@
         <xdr:cNvPr id="23" name="直接箭头连接符 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2131,7 +2189,7 @@
         <xdr:cNvPr id="25" name="直接箭头连接符 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2184,7 +2242,7 @@
         <xdr:cNvPr id="28" name="直接箭头连接符 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2237,7 +2295,7 @@
         <xdr:cNvPr id="32" name="直接箭头连接符 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2290,7 +2348,7 @@
         <xdr:cNvPr id="34" name="直接箭头连接符 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2343,7 +2401,7 @@
         <xdr:cNvPr id="38" name="直接箭头连接符 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2396,7 +2454,7 @@
         <xdr:cNvPr id="39" name="直接箭头连接符 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2449,7 +2507,7 @@
         <xdr:cNvPr id="58" name="直接箭头连接符 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2502,7 +2560,7 @@
         <xdr:cNvPr id="59" name="直接箭头连接符 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2555,7 +2613,7 @@
         <xdr:cNvPr id="60" name="直接箭头连接符 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2608,7 +2666,7 @@
         <xdr:cNvPr id="66" name="直接箭头连接符 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2661,7 +2719,7 @@
         <xdr:cNvPr id="20" name="直接箭头连接符 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2714,7 +2772,7 @@
         <xdr:cNvPr id="22" name="直接箭头连接符 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2767,7 +2825,7 @@
         <xdr:cNvPr id="26" name="直接箭头连接符 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2820,7 +2878,7 @@
         <xdr:cNvPr id="54" name="直接箭头连接符 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2873,7 +2931,7 @@
         <xdr:cNvPr id="55" name="直接箭头连接符 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2926,7 +2984,7 @@
         <xdr:cNvPr id="57" name="直接箭头连接符 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2979,7 +3037,7 @@
         <xdr:cNvPr id="64" name="直接箭头连接符 63">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3032,7 +3090,7 @@
         <xdr:cNvPr id="65" name="直接箭头连接符 64">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3085,7 +3143,7 @@
         <xdr:cNvPr id="67" name="直接箭头连接符 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3138,7 +3196,7 @@
         <xdr:cNvPr id="68" name="直接箭头连接符 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3191,7 +3249,7 @@
         <xdr:cNvPr id="70" name="直接箭头连接符 69">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3244,7 +3302,7 @@
         <xdr:cNvPr id="71" name="直接箭头连接符 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3297,7 +3355,7 @@
         <xdr:cNvPr id="72" name="直接箭头连接符 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3350,7 +3408,7 @@
         <xdr:cNvPr id="73" name="直接箭头连接符 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3403,7 +3461,7 @@
         <xdr:cNvPr id="74" name="直接箭头连接符 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000053000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3456,7 +3514,7 @@
         <xdr:cNvPr id="75" name="直接箭头连接符 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3509,7 +3567,7 @@
         <xdr:cNvPr id="76" name="直接箭头连接符 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3562,7 +3620,7 @@
         <xdr:cNvPr id="77" name="直接箭头连接符 76">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3615,7 +3673,7 @@
         <xdr:cNvPr id="78" name="直接箭头连接符 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3668,7 +3726,7 @@
         <xdr:cNvPr id="79" name="直接箭头连接符 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3721,7 +3779,7 @@
         <xdr:cNvPr id="80" name="直接箭头连接符 79">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3774,7 +3832,7 @@
         <xdr:cNvPr id="52" name="直接箭头连接符 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3827,7 +3885,7 @@
         <xdr:cNvPr id="61" name="直接箭头连接符 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3880,7 +3938,7 @@
         <xdr:cNvPr id="62" name="直接箭头连接符 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3933,7 +3991,7 @@
         <xdr:cNvPr id="69" name="直接箭头连接符 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3986,7 +4044,7 @@
         <xdr:cNvPr id="81" name="直接箭头连接符 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4039,7 +4097,7 @@
         <xdr:cNvPr id="82" name="直接箭头连接符 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4092,7 +4150,7 @@
         <xdr:cNvPr id="86" name="直接箭头连接符 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4145,7 +4203,7 @@
         <xdr:cNvPr id="87" name="直接箭头连接符 86">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4198,7 +4256,7 @@
         <xdr:cNvPr id="88" name="直接箭头连接符 87">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4437,7 +4495,7 @@
         <xdr:cNvPr id="83" name="直接箭头连接符 82">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4490,7 +4548,7 @@
         <xdr:cNvPr id="85" name="直接箭头连接符 84">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4543,7 +4601,7 @@
         <xdr:cNvPr id="90" name="直接箭头连接符 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4596,7 +4654,7 @@
         <xdr:cNvPr id="91" name="直接箭头连接符 90">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4649,7 +4707,7 @@
         <xdr:cNvPr id="95" name="直接箭头连接符 94">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4702,7 +4760,7 @@
         <xdr:cNvPr id="103" name="直接箭头连接符 102">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4755,7 +4813,7 @@
         <xdr:cNvPr id="84" name="直接箭头连接符 83">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4808,7 +4866,7 @@
         <xdr:cNvPr id="89" name="直接箭头连接符 88">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4861,7 +4919,7 @@
         <xdr:cNvPr id="92" name="直接箭头连接符 91">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4914,7 +4972,7 @@
         <xdr:cNvPr id="94" name="直接箭头连接符 93">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4995,7 +5053,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5030,7 +5088,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5239,10 +5297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S213"/>
+  <dimension ref="A2:S210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B169" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O186" sqref="O186"/>
+    <sheetView tabSelected="1" topLeftCell="B144" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q173" sqref="Q173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7099,7 +7157,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="145" spans="9:15" x14ac:dyDescent="0.15">
+    <row r="145" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I145" s="11" t="s">
         <v>217</v>
       </c>
@@ -7110,12 +7168,12 @@
         <v>217</v>
       </c>
     </row>
-    <row r="146" spans="9:15" x14ac:dyDescent="0.15">
+    <row r="146" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I146" s="11"/>
       <c r="K146" s="11"/>
       <c r="O146" s="11"/>
     </row>
-    <row r="147" spans="9:15" x14ac:dyDescent="0.15">
+    <row r="147" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I147" s="11" t="s">
         <v>236</v>
       </c>
@@ -7126,12 +7184,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="148" spans="9:15" x14ac:dyDescent="0.15">
+    <row r="148" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I148" s="11"/>
       <c r="K148" s="11"/>
       <c r="O148" s="11"/>
     </row>
-    <row r="149" spans="9:15" x14ac:dyDescent="0.15">
+    <row r="149" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I149" s="11" t="s">
         <v>225</v>
       </c>
@@ -7142,7 +7200,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="150" spans="9:15" x14ac:dyDescent="0.15">
+    <row r="150" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I150" s="12" t="s">
         <v>226</v>
       </c>
@@ -7153,7 +7211,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="151" spans="9:15" x14ac:dyDescent="0.15">
+    <row r="151" spans="2:15" x14ac:dyDescent="0.15">
       <c r="I151" s="12" t="s">
         <v>239</v>
       </c>
@@ -7164,22 +7222,52 @@
         <v>274</v>
       </c>
     </row>
-    <row r="155" spans="9:15" ht="27" x14ac:dyDescent="0.15">
+    <row r="155" spans="2:15" ht="27" x14ac:dyDescent="0.15">
       <c r="K155" s="16" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="156" spans="9:15" x14ac:dyDescent="0.15">
+    <row r="156" spans="2:15" x14ac:dyDescent="0.15">
       <c r="K156" t="s">
         <v>262</v>
       </c>
     </row>
+    <row r="159" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B159" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="162" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B162" s="33" t="s">
+        <v>346</v>
+      </c>
+      <c r="C162" s="33"/>
+      <c r="G162" s="31" t="s">
+        <v>344</v>
+      </c>
+      <c r="H162" s="32"/>
+      <c r="I162" s="32" t="s">
+        <v>341</v>
+      </c>
+      <c r="J162" s="32"/>
+      <c r="K162" s="32" t="s">
+        <v>338</v>
+      </c>
+      <c r="L162" s="32"/>
+      <c r="M162" s="32" t="s">
+        <v>343</v>
+      </c>
+      <c r="N162" s="32"/>
+      <c r="O162" s="32" t="s">
+        <v>342</v>
+      </c>
+    </row>
     <row r="164" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B164" t="s">
-        <v>308</v>
+        <v>340</v>
       </c>
       <c r="G164" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I164" s="18" t="s">
         <v>282</v>
@@ -7196,16 +7284,16 @@
     </row>
     <row r="165" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B165" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D165" s="27" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="K165" t="s">
         <v>288</v>
       </c>
       <c r="M165" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="O165" s="25" t="s">
         <v>290</v>
@@ -7213,16 +7301,16 @@
     </row>
     <row r="166" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B166" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D166" s="30" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="K166" t="s">
         <v>289</v>
       </c>
       <c r="M166" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="O166" s="22" t="s">
         <v>295</v>
@@ -7230,37 +7318,37 @@
     </row>
     <row r="167" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B167" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D167" s="27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="168" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B168" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D168" s="27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="169" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B169" t="s">
-        <v>328</v>
+        <v>339</v>
       </c>
       <c r="D169" s="27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="170" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B170" t="s">
+        <v>326</v>
+      </c>
+      <c r="D170" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="G170" t="s">
         <v>329</v>
-      </c>
-      <c r="D170" s="27" t="s">
-        <v>309</v>
-      </c>
-      <c r="G170" t="s">
-        <v>332</v>
       </c>
       <c r="I170" s="20" t="s">
         <v>283</v>
@@ -7280,7 +7368,7 @@
         <v>288</v>
       </c>
       <c r="M171" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="O171" s="25" t="s">
         <v>290</v>
@@ -7291,7 +7379,7 @@
         <v>289</v>
       </c>
       <c r="M172" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="O172" s="26" t="s">
         <v>290</v>
@@ -7299,7 +7387,7 @@
     </row>
     <row r="176" spans="2:15" x14ac:dyDescent="0.15">
       <c r="G176" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I176" s="21" t="s">
         <v>284</v>
@@ -7308,7 +7396,7 @@
         <v>291</v>
       </c>
       <c r="M176" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="O176" s="22" t="s">
         <v>295</v>
@@ -7316,7 +7404,7 @@
     </row>
     <row r="181" spans="7:15" x14ac:dyDescent="0.15">
       <c r="G181" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I181" s="22" t="s">
         <v>285</v>
@@ -7333,21 +7421,21 @@
     </row>
     <row r="182" spans="7:15" x14ac:dyDescent="0.15">
       <c r="G182" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K182" t="s">
         <v>297</v>
       </c>
       <c r="M182" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O182" s="21" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="183" spans="7:15" x14ac:dyDescent="0.15">
       <c r="G183" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="K183" t="s">
         <v>298</v>
@@ -7367,16 +7455,16 @@
         <v>304</v>
       </c>
       <c r="O184" s="25" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="185" spans="7:15" x14ac:dyDescent="0.15">
       <c r="K185" s="28" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="L185" s="28"/>
       <c r="M185" s="28" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="N185" s="28"/>
       <c r="O185" s="29" t="s">
@@ -7388,7 +7476,7 @@
         <v>300</v>
       </c>
       <c r="M186" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="O186" s="23" t="s">
         <v>306</v>
@@ -7396,7 +7484,7 @@
     </row>
     <row r="189" spans="7:15" x14ac:dyDescent="0.15">
       <c r="G189" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I189" s="24" t="s">
         <v>286</v>
@@ -7415,7 +7503,7 @@
     </row>
     <row r="190" spans="7:15" x14ac:dyDescent="0.15">
       <c r="G190" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K190" s="28" t="s">
         <v>297</v>
@@ -7431,7 +7519,7 @@
     </row>
     <row r="191" spans="7:15" x14ac:dyDescent="0.15">
       <c r="G191" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="K191" t="s">
         <v>298</v>
@@ -7456,11 +7544,11 @@
     </row>
     <row r="193" spans="2:15" x14ac:dyDescent="0.15">
       <c r="K193" s="28" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="L193" s="28"/>
       <c r="M193" s="28" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="N193" s="28"/>
       <c r="O193" s="29" t="s">
@@ -7472,35 +7560,90 @@
         <v>289</v>
       </c>
       <c r="M194" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O194" s="25" t="s">
         <v>290</v>
       </c>
     </row>
+    <row r="198" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B198" s="33" t="s">
+        <v>345</v>
+      </c>
+      <c r="C198" s="33"/>
+      <c r="D198" s="33"/>
+    </row>
+    <row r="199" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B199" t="s">
+        <v>322</v>
+      </c>
+      <c r="D199" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="G199" t="s">
+        <v>327</v>
+      </c>
+      <c r="I199" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="K199" t="s">
+        <v>296</v>
+      </c>
+      <c r="M199" t="s">
+        <v>292</v>
+      </c>
+      <c r="O199" s="25" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="200" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="B200" t="s">
+        <v>323</v>
+      </c>
+      <c r="D200" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="K200" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="L200" s="28"/>
+      <c r="M200" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="N200" s="28"/>
+      <c r="O200" s="29" t="s">
+        <v>290</v>
+      </c>
+    </row>
     <row r="201" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B201" t="s">
-        <v>312</v>
+        <v>324</v>
+      </c>
+      <c r="D201" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="K201" t="s">
+        <v>298</v>
+      </c>
+      <c r="M201" t="s">
+        <v>303</v>
+      </c>
+      <c r="O201" s="25" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="202" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B202" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D202" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="G202" t="s">
-        <v>330</v>
-      </c>
-      <c r="I202" s="24" t="s">
-        <v>286</v>
-      </c>
       <c r="K202" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="M202" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="O202" s="25" t="s">
         <v>290</v>
@@ -7508,21 +7651,19 @@
     </row>
     <row r="203" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B203" t="s">
-        <v>325</v>
+        <v>339</v>
       </c>
       <c r="D203" s="23" t="s">
-        <v>337</v>
-      </c>
-      <c r="K203" s="28" t="s">
-        <v>297</v>
-      </c>
-      <c r="L203" s="28"/>
-      <c r="M203" s="28" t="s">
-        <v>302</v>
-      </c>
-      <c r="N203" s="28"/>
-      <c r="O203" s="29" t="s">
-        <v>290</v>
+        <v>306</v>
+      </c>
+      <c r="K203" t="s">
+        <v>289</v>
+      </c>
+      <c r="M203" t="s">
+        <v>311</v>
+      </c>
+      <c r="O203" s="22" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="204" spans="2:15" x14ac:dyDescent="0.15">
@@ -7532,119 +7673,68 @@
       <c r="D204" s="23" t="s">
         <v>306</v>
       </c>
-      <c r="K204" t="s">
+    </row>
+    <row r="206" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="G206" t="s">
+        <v>328</v>
+      </c>
+      <c r="I206" s="22" t="s">
+        <v>310</v>
+      </c>
+      <c r="K206" t="s">
+        <v>296</v>
+      </c>
+      <c r="M206" t="s">
+        <v>292</v>
+      </c>
+      <c r="O206" s="25" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="207" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="G207" t="s">
+        <v>336</v>
+      </c>
+      <c r="K207" t="s">
+        <v>297</v>
+      </c>
+      <c r="M207" t="s">
+        <v>335</v>
+      </c>
+      <c r="O207" s="25" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="208" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="K208" t="s">
         <v>298</v>
       </c>
-      <c r="M204" t="s">
+      <c r="M208" t="s">
         <v>303</v>
       </c>
-      <c r="O204" s="25" t="s">
+      <c r="O208" s="25" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="205" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B205" t="s">
-        <v>327</v>
-      </c>
-      <c r="D205" s="23" t="s">
-        <v>306</v>
-      </c>
-      <c r="K205" t="s">
+    <row r="209" spans="11:15" x14ac:dyDescent="0.15">
+      <c r="K209" t="s">
         <v>299</v>
       </c>
-      <c r="M205" t="s">
+      <c r="M209" t="s">
         <v>304</v>
-      </c>
-      <c r="O205" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="206" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B206" t="s">
-        <v>328</v>
-      </c>
-      <c r="D206" s="23" t="s">
-        <v>306</v>
-      </c>
-      <c r="K206" t="s">
-        <v>289</v>
-      </c>
-      <c r="M206" t="s">
-        <v>313</v>
-      </c>
-      <c r="O206" s="22" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="207" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B207" t="s">
-        <v>329</v>
-      </c>
-      <c r="D207" s="23" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="209" spans="7:15" x14ac:dyDescent="0.15">
-      <c r="G209" t="s">
-        <v>331</v>
-      </c>
-      <c r="I209" s="22" t="s">
-        <v>311</v>
-      </c>
-      <c r="K209" t="s">
-        <v>296</v>
-      </c>
-      <c r="M209" t="s">
-        <v>292</v>
       </c>
       <c r="O209" s="25" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="210" spans="7:15" x14ac:dyDescent="0.15">
-      <c r="G210" t="s">
-        <v>339</v>
-      </c>
+    <row r="210" spans="11:15" x14ac:dyDescent="0.15">
       <c r="K210" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="M210" t="s">
-        <v>338</v>
+        <v>309</v>
       </c>
       <c r="O210" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="211" spans="7:15" x14ac:dyDescent="0.15">
-      <c r="K211" t="s">
-        <v>298</v>
-      </c>
-      <c r="M211" t="s">
-        <v>303</v>
-      </c>
-      <c r="O211" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="212" spans="7:15" x14ac:dyDescent="0.15">
-      <c r="K212" t="s">
-        <v>299</v>
-      </c>
-      <c r="M212" t="s">
-        <v>304</v>
-      </c>
-      <c r="O212" s="25" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="213" spans="7:15" x14ac:dyDescent="0.15">
-      <c r="K213" t="s">
-        <v>289</v>
-      </c>
-      <c r="M213" t="s">
-        <v>310</v>
-      </c>
-      <c r="O213" s="25" t="s">
         <v>290</v>
       </c>
     </row>

</xml_diff>